<commit_message>
atualizando estrutura de pastas
</commit_message>
<xml_diff>
--- a/dicionario_dados/template1.xlsx
+++ b/dicionario_dados/template1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e404f7af6d399db5/@SATC_Aula/202302/BDII/TERCA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codigos\projeto-bd2-satc\dicionario_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{5A897C1D-2E5E-4C7F-B782-B7F57F8C8B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75050446-9156-43AA-AFAD-B45741CD4360}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEC94C6-ACA5-4C7C-8D61-130F0B6D9D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>int</t>
   </si>
   <si>
-    <t>1 – sem limite</t>
-  </si>
-  <si>
     <t>NOT NULL</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Idx_dt_avaliacao</t>
+  </si>
+  <si>
+    <t>1 – 2.147.483.647</t>
   </si>
 </sst>
 </file>
@@ -140,14 +140,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1" tint="0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFA6A6A6"/>
+      <color theme="1" tint="0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -208,7 +208,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -220,19 +226,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -251,9 +244,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -291,7 +284,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -397,7 +390,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -539,7 +532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,69 +540,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -624,191 +618,198 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="4"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="8"/>
       <c r="F14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>14</v>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="4"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="8"/>
       <c r="F16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:H15"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="B1:H1"/>
@@ -822,14 +823,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:H15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>